<commit_message>
more renames, dialog api bootstrap
</commit_message>
<xml_diff>
--- a/manifest/bin/Debug/Book1.xlsx
+++ b/manifest/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R4919ad4f90cf4443"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R6ad9181617a64d52"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="700" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rc4458a9ccc6f45cd"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R39e1e842fb2243a8"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{5aaa87e5-15ab-48d8-8334-18dcb0fe2f56}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4dd2d3bf-1d40-4731-8800-aba0faf81c23}">
   <we:reference id="ef16b601-2bed-45d3-8ecb-209e9042df76" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>